<commit_message>
Week 7 Daily updates - 2 October
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tricia\Documents\GitHub\project-g4t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F11D9B8-1C84-48A5-AD19-21146DDFB2AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EA0F45-A031-47E9-8CD2-6A5A0B11BD47}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="112">
   <si>
     <t>Question</t>
   </si>
@@ -343,6 +343,27 @@
   </si>
   <si>
     <t>Week 5: 30 September to 6 October</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meet to discuss iterations and prep for PM review </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prep for Pm review </t>
+  </si>
+  <si>
+    <t>Validations for bootstrap. Test and debugged validations.</t>
+  </si>
+  <si>
+    <t>Code delete.php, deleteDAO and delete processing</t>
+  </si>
+  <si>
+    <t>Revise PM Review presentation slides</t>
+  </si>
+  <si>
+    <t>Meet to discuss slides and prepare for PM review</t>
+  </si>
+  <si>
+    <t>Bug metrics</t>
   </si>
 </sst>
 </file>
@@ -439,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -457,6 +478,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -470,20 +506,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,9 +794,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V6" sqref="V6"/>
+      <selection pane="topRight" activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -793,21 +817,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
       <c r="J1" s="6" t="s">
         <v>46</v>
       </c>
@@ -816,23 +840,23 @@
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="15" t="s">
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.4">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
@@ -884,1040 +908,1085 @@
       <c r="S2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="T2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="U2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="V2" s="16" t="s">
+      <c r="V2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="W2" s="16" t="s">
+      <c r="W2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="16" t="s">
+      <c r="X2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="16" t="s">
+      <c r="Y2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="16" t="s">
+      <c r="Z2" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="12" t="s">
+      <c r="F3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="12" t="s">
+      <c r="I3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="12" t="s">
+      <c r="L3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="P3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="12" t="s">
+      <c r="P3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="T3" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="U3" s="14" t="s">
-        <v>19</v>
+      <c r="U3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="9"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="12" t="s">
+      <c r="E4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="13" t="s">
+      <c r="H4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="12" t="s">
+      <c r="J4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="O4" s="13" t="s">
+      <c r="O4" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="P4" s="13" t="s">
+      <c r="P4" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="Q4" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="R4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S4" s="12" t="s">
+      <c r="R4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="T4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="U4" s="14" t="s">
+      <c r="T4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="U4" s="9" t="s">
         <v>100</v>
       </c>
+      <c r="V4" s="7" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="9"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="13" t="s">
+      <c r="C5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="12" t="s">
+      <c r="J5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="P5" s="13" t="s">
+      <c r="N5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="Q5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="R5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="S5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="T5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="U5" s="14" t="s">
+      <c r="Q5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="U5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="V5" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="13" t="s">
+      <c r="E6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="12" t="s">
+      <c r="I6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="O6" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="P6" s="13" t="s">
+      <c r="P6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="Q6" s="12" t="s">
+      <c r="Q6" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="R6" s="12" t="s">
+      <c r="R6" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="S6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T6" s="14" t="s">
+      <c r="S6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T6" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="U6" s="14" t="s">
-        <v>19</v>
+      <c r="U6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="V6" s="17" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="9"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="12" t="s">
+      <c r="D7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="13" t="s">
+      <c r="H7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="M7" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="N7" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="O7" s="13" t="s">
+      <c r="O7" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="P7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q7" s="12" t="s">
+      <c r="P7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="R7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S7" s="12" t="s">
+      <c r="R7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S7" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="T7" s="14" t="s">
+      <c r="T7" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="U7" s="14" t="s">
+      <c r="U7" s="9" t="s">
         <v>102</v>
       </c>
+      <c r="V7" s="17" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="9"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="12" t="s">
+      <c r="C8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="N8" s="12" t="s">
+      <c r="N8" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="O8" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="P8" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="R8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="S8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="T8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="U8" s="14" t="s">
+      <c r="O8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="U8" s="9" t="s">
         <v>103</v>
       </c>
+      <c r="V8" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="12" t="s">
+      <c r="C9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="12" t="s">
+      <c r="E9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="12" t="s">
+      <c r="I9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="L9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O9" s="13" t="s">
+      <c r="L9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="P9" s="13" t="s">
+      <c r="P9" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="Q9" s="12" t="s">
+      <c r="Q9" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="R9" s="12" t="s">
+      <c r="R9" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="S9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T9" s="14" t="s">
+      <c r="S9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T9" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="U9" s="14" t="s">
+      <c r="U9" s="9" t="s">
         <v>96</v>
       </c>
+      <c r="V9" s="17" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="9"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="12" t="s">
+      <c r="D10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="12" t="s">
+      <c r="F10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="13" t="s">
+      <c r="H10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N10" s="12" t="s">
+      <c r="J10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="O10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="P10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q10" s="12" t="s">
+      <c r="O10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="R10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S10" s="12" t="s">
+      <c r="R10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S10" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="T10" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="U10" s="14" t="s">
+      <c r="T10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="U10" s="9" t="s">
         <v>97</v>
       </c>
+      <c r="V10" s="17" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="9"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="O11" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="P11" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="R11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="S11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="T11" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="U11" s="13" t="s">
+      <c r="C11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="T11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="U11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="V11" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="12" t="s">
+      <c r="E12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" s="12" t="s">
+      <c r="I12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N12" s="12" t="s">
+      <c r="L12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="O12" s="13" t="s">
+      <c r="O12" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="P12" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q12" s="12" t="s">
+      <c r="P12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="R12" s="12" t="s">
+      <c r="R12" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="S12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T12" s="14" t="s">
+      <c r="S12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T12" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="U12" s="13" t="s">
-        <v>19</v>
+      <c r="U12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="9"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="12" t="s">
+      <c r="D13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="13" t="s">
+      <c r="H13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" s="12" t="s">
+      <c r="J13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="N13" s="12" t="s">
+      <c r="N13" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="O13" s="13" t="s">
+      <c r="O13" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="P13" s="13" t="s">
+      <c r="P13" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="Q13" s="12" t="s">
+      <c r="Q13" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="R13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S13" s="12" t="s">
+      <c r="R13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S13" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="T13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="U13" s="13" t="s">
+      <c r="T13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="U13" s="8" t="s">
         <v>98</v>
       </c>
+      <c r="V13" s="17" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="9"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="12" t="s">
+      <c r="C14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="O14" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="P14" s="13" t="s">
+      <c r="H14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P14" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Q14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="R14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="S14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="T14" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="U14" s="13" t="s">
+      <c r="Q14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="R14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="S14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="T14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="U14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="V14" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="12" t="s">
+      <c r="C15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="12" t="s">
+      <c r="E15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I15" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="12" t="s">
+      <c r="I15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="M15" s="12" t="s">
+      <c r="M15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="N15" s="12" t="s">
+      <c r="N15" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="O15" s="13" t="s">
+      <c r="O15" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="P15" s="13" t="s">
+      <c r="P15" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="Q15" s="12" t="s">
+      <c r="Q15" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="R15" s="12" t="s">
+      <c r="R15" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="S15" s="12" t="s">
+      <c r="S15" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="T15" s="14" t="s">
+      <c r="T15" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="U15" s="14" t="s">
+      <c r="U15" s="9" t="s">
         <v>99</v>
       </c>
+      <c r="V15" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="9"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="12" t="s">
+      <c r="D16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="13" t="s">
+      <c r="H16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="L16" s="12" t="s">
+      <c r="L16" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="M16" s="12" t="s">
+      <c r="M16" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N16" s="12" t="s">
+      <c r="N16" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="O16" s="13" t="s">
+      <c r="O16" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="P16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q16" s="12" t="s">
+      <c r="P16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q16" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="R16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S16" s="12" t="s">
+      <c r="R16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S16" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="T16" s="14" t="s">
+      <c r="T16" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="U16" s="14" t="s">
+      <c r="U16" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="9"/>
+      <c r="V16" s="17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="14"/>
       <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="12" t="s">
+      <c r="C17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="12" t="s">
+      <c r="G17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="K17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M17" s="12" t="s">
+      <c r="K17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="N17" s="12" t="s">
+      <c r="N17" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="O17" s="13" t="s">
+      <c r="O17" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="P17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="R17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="S17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="T17" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="U17" s="14" t="s">
+      <c r="P17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="T17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="U17" s="9" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+      <c r="V17" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A25" s="1"/>
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A27" s="1"/>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A28" s="1"/>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A29" s="1"/>
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" s="1"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" s="1"/>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:22" ht="15" x14ac:dyDescent="0.4">
       <c r="A32" s="1"/>
       <c r="B32" s="3"/>
     </row>

</xml_diff>

<commit_message>
Week 7 Daily Updates - 4 October
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tricia\Documents\GitHub\project-g4t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF04AA3E-BEC8-411C-ABEB-B4F61D1AC148}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD1077A-8462-448D-8EE5-E122B061357A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="124">
   <si>
     <t>Question</t>
   </si>
@@ -385,6 +385,21 @@
   </si>
   <si>
     <t>Deploying to AWS</t>
+  </si>
+  <si>
+    <t>PM review with the team</t>
+  </si>
+  <si>
+    <t>PM Review with team, Scheduling</t>
+  </si>
+  <si>
+    <t>Pair programming with Casper for add bid validations</t>
+  </si>
+  <si>
+    <t>Pair programming with Tricia for add bid validations</t>
+  </si>
+  <si>
+    <t>Fixed deployment issues on AWS and PM review with team</t>
   </si>
 </sst>
 </file>
@@ -499,6 +514,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -508,17 +527,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,8 +820,8 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D6" sqref="D6"/>
+      <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -829,21 +844,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
       <c r="J1" s="5" t="s">
         <v>46</v>
       </c>
@@ -852,23 +867,23 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="9" t="s">
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.4">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
@@ -943,7 +958,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1006,18 +1021,20 @@
       <c r="U3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="V3" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="W3" s="15" t="s">
+      <c r="W3" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
+      <c r="X3" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="16"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1078,18 +1095,20 @@
       <c r="U4" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="V4" s="15" t="s">
+      <c r="V4" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="W4" s="15" t="s">
+      <c r="W4" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
+      <c r="X4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="16"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1156,12 +1175,14 @@
       <c r="W5" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
+      <c r="X5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1224,18 +1245,20 @@
       <c r="U6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="V6" s="15" t="s">
+      <c r="V6" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="W6" s="15" t="s">
+      <c r="W6" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="14"/>
-      <c r="Z6" s="14"/>
+      <c r="X6" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="16"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1296,18 +1319,20 @@
       <c r="U7" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="V7" s="15" t="s">
+      <c r="V7" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="W7" s="15" t="s">
+      <c r="W7" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="14"/>
+      <c r="X7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="16"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1374,12 +1399,14 @@
       <c r="W8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
-      <c r="Z8" s="14"/>
+      <c r="X8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1442,18 +1469,20 @@
       <c r="U9" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="V9" s="15" t="s">
+      <c r="V9" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="W9" s="15" t="s">
+      <c r="W9" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
+      <c r="X9" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="16"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1514,18 +1543,20 @@
       <c r="U10" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="V10" s="15" t="s">
+      <c r="V10" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="W10" s="15" t="s">
+      <c r="W10" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="14"/>
-      <c r="Z10" s="14"/>
+      <c r="X10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="16"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1586,18 +1617,20 @@
       <c r="U11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V11" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="W11" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="14"/>
+      <c r="V11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="W11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="X11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1660,18 +1693,20 @@
       <c r="U12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="V12" s="15" t="s">
+      <c r="V12" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="W12" s="15" t="s">
+      <c r="W12" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="14"/>
+      <c r="X12" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="16"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1732,18 +1767,20 @@
       <c r="U13" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="V13" s="15" t="s">
+      <c r="V13" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="W13" s="15" t="s">
+      <c r="W13" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
+      <c r="X13" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="16"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1804,18 +1841,20 @@
       <c r="U14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V14" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="W14" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="14"/>
+      <c r="V14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="W14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="X14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1878,18 +1917,20 @@
       <c r="U15" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="V15" s="15" t="s">
+      <c r="V15" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="W15" s="15" t="s">
+      <c r="W15" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="X15" s="14"/>
-      <c r="Y15" s="14"/>
-      <c r="Z15" s="14"/>
+      <c r="X15" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="16"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1950,18 +1991,20 @@
       <c r="U16" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="V16" s="15" t="s">
+      <c r="V16" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="W16" s="15" t="s">
+      <c r="W16" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="X16" s="14"/>
-      <c r="Y16" s="14"/>
-      <c r="Z16" s="14"/>
+      <c r="X16" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
     </row>
     <row r="17" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="16"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
@@ -2025,12 +2068,14 @@
       <c r="V17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="W17" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="X17" s="14"/>
-      <c r="Y17" s="14"/>
-      <c r="Z17" s="14"/>
+      <c r="W17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="X17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
     </row>
     <row r="18" spans="1:26" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" s="1"/>

</xml_diff>

<commit_message>
Update slides and daily updates
Week 9 Daily Updates - 16 Oct, include critical path
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tricia\Documents\GitHub\project-g4t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325D107A-2B37-4467-82AB-912C92E68A56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47ADF91-3F35-4E37-91EC-D1A4AF5ED7F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2805" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2304" uniqueCount="176">
   <si>
     <t>Question</t>
   </si>
@@ -538,6 +538,24 @@
   </si>
   <si>
     <t xml:space="preserve">Sharing rounds logic with Celine/ Pair Programming </t>
+  </si>
+  <si>
+    <t>Debugging, delete and update web service</t>
+  </si>
+  <si>
+    <t>meeting for debugging, testing, aws deployment and slides</t>
+  </si>
+  <si>
+    <t>meeting for debugging, testing, aws deployment and presentation slides</t>
+  </si>
+  <si>
+    <t>testing, slides</t>
+  </si>
+  <si>
+    <t>Testing - login and add bid function (manual). Bugs logged in bug metrics.</t>
+  </si>
+  <si>
+    <t>Meeting for debugging, testing, aws deployment and slides</t>
   </si>
 </sst>
 </file>
@@ -708,7 +726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -778,17 +796,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -808,17 +820,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1105,9 +1135,9 @@
   </sheetPr>
   <dimension ref="A1:AN1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
       <pane xSplit="2" topLeftCell="AG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AI12" sqref="AI12"/>
+      <selection pane="topRight" activeCell="AK24" sqref="AK24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1119,27 +1149,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="34" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="34" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="32" t="s">
         <v>124</v>
       </c>
       <c r="N1" s="37"/>
@@ -1148,37 +1178,37 @@
       <c r="Q1" s="37"/>
       <c r="R1" s="37"/>
       <c r="S1" s="38"/>
-      <c r="T1" s="31" t="s">
+      <c r="T1" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="31" t="s">
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="31" t="s">
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="33"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="31"/>
     </row>
     <row r="2" spans="1:40" ht="15" x14ac:dyDescent="0.4">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="23" t="s">
         <v>6</v>
       </c>
@@ -1295,7 +1325,7 @@
       </c>
     </row>
     <row r="3" spans="1:40" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="35" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1397,17 +1427,19 @@
       <c r="AH3" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="AI3" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ3" s="9"/>
+      <c r="AI3" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ3" s="43" t="s">
+        <v>170</v>
+      </c>
       <c r="AK3" s="9"/>
       <c r="AL3" s="9"/>
       <c r="AM3" s="9"/>
       <c r="AN3" s="10"/>
     </row>
     <row r="4" spans="1:40" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="28"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1507,17 +1539,19 @@
       <c r="AH4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="AI4" s="39" t="s">
+      <c r="AI4" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="AJ4" s="9"/>
+      <c r="AJ4" s="43" t="s">
+        <v>171</v>
+      </c>
       <c r="AK4" s="9"/>
       <c r="AL4" s="9"/>
       <c r="AM4" s="9"/>
       <c r="AN4" s="10"/>
     </row>
     <row r="5" spans="1:40" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="28"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1617,17 +1651,19 @@
       <c r="AH5" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="AI5" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="AJ5" s="9"/>
+      <c r="AI5" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ5" s="41" t="s">
+        <v>19</v>
+      </c>
       <c r="AK5" s="9"/>
       <c r="AL5" s="9"/>
       <c r="AM5" s="9"/>
       <c r="AN5" s="10"/>
     </row>
     <row r="6" spans="1:40" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="35" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1732,14 +1768,16 @@
       <c r="AI6" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="AJ6" s="9"/>
+      <c r="AJ6" s="43" t="s">
+        <v>173</v>
+      </c>
       <c r="AK6" s="9"/>
       <c r="AL6" s="9"/>
       <c r="AM6" s="9"/>
       <c r="AN6" s="10"/>
     </row>
     <row r="7" spans="1:40" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="28"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1839,17 +1877,19 @@
       <c r="AH7" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="AI7" s="39" t="s">
+      <c r="AI7" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="AJ7" s="9"/>
+      <c r="AJ7" s="43" t="s">
+        <v>171</v>
+      </c>
       <c r="AK7" s="9"/>
       <c r="AL7" s="9"/>
       <c r="AM7" s="9"/>
       <c r="AN7" s="10"/>
     </row>
     <row r="8" spans="1:40" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="28"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1949,17 +1989,19 @@
       <c r="AH8" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="AI8" s="39" t="s">
+      <c r="AI8" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="AJ8" s="9"/>
+      <c r="AJ8" s="42" t="s">
+        <v>19</v>
+      </c>
       <c r="AK8" s="9"/>
       <c r="AL8" s="9"/>
       <c r="AM8" s="9"/>
       <c r="AN8" s="10"/>
     </row>
     <row r="9" spans="1:40" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -2061,17 +2103,19 @@
       <c r="AH9" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="AI9" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ9" s="9"/>
+      <c r="AI9" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ9" s="43" t="s">
+        <v>170</v>
+      </c>
       <c r="AK9" s="9"/>
       <c r="AL9" s="9"/>
       <c r="AM9" s="9"/>
       <c r="AN9" s="10"/>
     </row>
     <row r="10" spans="1:40" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="28"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -2171,17 +2215,19 @@
       <c r="AH10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="AI10" s="39" t="s">
+      <c r="AI10" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="AJ10" s="9"/>
+      <c r="AJ10" s="43" t="s">
+        <v>171</v>
+      </c>
       <c r="AK10" s="9"/>
       <c r="AL10" s="9"/>
       <c r="AM10" s="9"/>
       <c r="AN10" s="10"/>
     </row>
     <row r="11" spans="1:40" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="28"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -2281,17 +2327,19 @@
       <c r="AH11" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="AI11" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="AJ11" s="9"/>
+      <c r="AI11" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ11" s="41" t="s">
+        <v>19</v>
+      </c>
       <c r="AK11" s="9"/>
       <c r="AL11" s="9"/>
       <c r="AM11" s="9"/>
       <c r="AN11" s="10"/>
     </row>
     <row r="12" spans="1:40" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="35" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -2396,14 +2444,16 @@
       <c r="AI12" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="AJ12" s="9"/>
+      <c r="AJ12" s="42" t="s">
+        <v>167</v>
+      </c>
       <c r="AK12" s="9"/>
       <c r="AL12" s="9"/>
       <c r="AM12" s="9"/>
       <c r="AN12" s="10"/>
     </row>
     <row r="13" spans="1:40" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -2506,14 +2556,16 @@
       <c r="AI13" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="AJ13" s="9"/>
+      <c r="AJ13" s="43" t="s">
+        <v>172</v>
+      </c>
       <c r="AK13" s="9"/>
       <c r="AL13" s="9"/>
       <c r="AM13" s="9"/>
       <c r="AN13" s="10"/>
     </row>
     <row r="14" spans="1:40" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="28"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -2616,14 +2668,16 @@
       <c r="AI14" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="AJ14" s="9"/>
+      <c r="AJ14" s="42" t="s">
+        <v>19</v>
+      </c>
       <c r="AK14" s="9"/>
       <c r="AL14" s="9"/>
       <c r="AM14" s="9"/>
       <c r="AN14" s="10"/>
     </row>
     <row r="15" spans="1:40" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="35" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -2725,17 +2779,19 @@
       <c r="AH15" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="AI15" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ15" s="9"/>
+      <c r="AI15" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ15" s="43" t="s">
+        <v>174</v>
+      </c>
       <c r="AK15" s="9"/>
       <c r="AL15" s="9"/>
       <c r="AM15" s="9"/>
       <c r="AN15" s="10"/>
     </row>
     <row r="16" spans="1:40" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="28"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -2835,17 +2891,19 @@
       <c r="AH16" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="AI16" s="39" t="s">
+      <c r="AI16" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="AJ16" s="9"/>
+      <c r="AJ16" s="43" t="s">
+        <v>175</v>
+      </c>
       <c r="AK16" s="9"/>
       <c r="AL16" s="9"/>
       <c r="AM16" s="9"/>
       <c r="AN16" s="10"/>
     </row>
     <row r="17" spans="1:40" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="28"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -2945,10 +3003,12 @@
       <c r="AH17" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI17" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="AJ17" s="12"/>
+      <c r="AI17" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ17" s="44" t="s">
+        <v>19</v>
+      </c>
       <c r="AK17" s="12"/>
       <c r="AL17" s="12"/>
       <c r="AM17" s="12"/>
@@ -6892,6 +6952,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="AH1:AN1"/>
     <mergeCell ref="AA1:AG1"/>
     <mergeCell ref="C1:E1"/>
@@ -6899,12 +6965,6 @@
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="M1:S1"/>
     <mergeCell ref="F1:L1"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>